<commit_message>
Added window switch for multiple case creation Changes to be committed: 	modified:   FACE REND/Resources/FACE_REND_Keywords.resource 	modified:   FACE REND/Resources/FACE_REND_Variables.resource 	modified:   FACE REND/Resources/FORM_FACE_REND.xlsx
</commit_message>
<xml_diff>
--- a/FACE REND/Resources/FORM_FACE_REND.xlsx
+++ b/FACE REND/Resources/FORM_FACE_REND.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marylou.delacerna\Documents\Projects\Auto-Projects\SLA\FACE REND\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marylou.delacerna\Documents\Projects\Auto-Projects\Solutions-Tracker\FACE REND\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8268F31D-E9FC-4DB5-907E-A1E229FF93F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D451A8-DA7D-4047-B095-9C4E8C13F2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19880" yWindow="-7710" windowWidth="28800" windowHeight="15500" activeTab="2" xr2:uid="{641C40FE-1C70-4854-B815-ADB73DBD8C9F}"/>
+    <workbookView xWindow="21170" yWindow="-8210" windowWidth="28800" windowHeight="15500" activeTab="2" xr2:uid="{641C40FE-1C70-4854-B815-ADB73DBD8C9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Service Classification" sheetId="1" r:id="rId1"/>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45F8AA8-088B-42D6-94EB-CF34A509C99A}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A45052-92E4-433A-AB75-440835C16B38}">
   <dimension ref="A1:H1081"/>
   <sheetViews>
-    <sheetView topLeftCell="A768" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L803" sqref="L803"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>